<commit_message>
tracking hydroprogress and updating reduction efficiencies.
</commit_message>
<xml_diff>
--- a/doc/LitReview/TyndallLab/practice_reduction_estimates.xlsx
+++ b/doc/LitReview/TyndallLab/practice_reduction_estimates.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnel\Documents\Project\G2G_supplyshed\doc\LitReview\TyndallLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE040AC1-1163-4ADC-A781-0A0117A7425C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DF8A1B-27DD-4D51-BD70-3793AFA0C4FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22185" windowHeight="12000" activeTab="6" xr2:uid="{2B4A4EA7-2393-4A3B-BE3A-A25348E227CC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22185" windowHeight="12000" activeTab="2" xr2:uid="{2B4A4EA7-2393-4A3B-BE3A-A25348E227CC}"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="13" r:id="rId1"/>
     <sheet name="CPcodes" sheetId="14" r:id="rId2"/>
-    <sheet name="unorganized" sheetId="16" r:id="rId3"/>
+    <sheet name="papers" sheetId="16" r:id="rId3"/>
     <sheet name="misc" sheetId="15" r:id="rId4"/>
     <sheet name="nrw" sheetId="1" r:id="rId5"/>
     <sheet name="farmpond" sheetId="12" r:id="rId6"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="121">
   <si>
     <t>Nutrient Removal Wetland</t>
   </si>
@@ -388,6 +388,18 @@
   </si>
   <si>
     <t>McCarty and Ritchie. 2002. Impact of soil movement on carbon sequestration in agricultural ecosystems</t>
+  </si>
+  <si>
+    <t>BARC, Maryland</t>
+  </si>
+  <si>
+    <t>Christensen et al.</t>
+  </si>
+  <si>
+    <t>riparian buffers; IBI</t>
+  </si>
+  <si>
+    <t>conservation cover; TN; TSS; ChlA</t>
   </si>
 </sst>
 </file>
@@ -464,10 +476,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -788,7 +800,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,7 +1365,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,10 +1482,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FC7F79-CEB3-432E-A3AB-3A5236BDCD48}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1548,6 +1560,34 @@
         <v>104</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9">
+        <v>2009</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10">
+        <v>2012</v>
+      </c>
+      <c r="C10" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1558,7 +1598,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:P2"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,8 +1606,8 @@
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="30.7109375" customWidth="1"/>
   </cols>
@@ -1579,14 +1619,14 @@
       <c r="B1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
       <c r="I1" s="3" t="s">
         <v>20</v>
       </c>
@@ -1648,10 +1688,10 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="9" t="s">
         <v>27</v>
       </c>
       <c r="P3" t="s">
@@ -1666,10 +1706,10 @@
       <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="9">
         <v>28</v>
       </c>
       <c r="P4" t="s">
@@ -1683,10 +1723,10 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="9">
         <v>42</v>
       </c>
       <c r="P5" t="s">
@@ -1700,10 +1740,10 @@
       <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="9">
         <v>9</v>
       </c>
       <c r="P6" t="s">
@@ -1717,10 +1757,10 @@
       <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="9">
         <v>41</v>
       </c>
       <c r="P7" t="s">
@@ -1761,16 +1801,16 @@
       <c r="B1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
       <c r="K1" s="4" t="s">
         <v>20</v>
       </c>
@@ -2045,8 +2085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D415F46-8A27-4B6E-B90B-AAD6F6C1F58A}">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2065,14 +2105,14 @@
       <c r="B1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
       <c r="I1" s="3" t="s">
         <v>20</v>
       </c>
@@ -2138,6 +2178,9 @@
       </c>
       <c r="J3">
         <v>1.5</v>
+      </c>
+      <c r="M3" t="s">
+        <v>117</v>
       </c>
       <c r="P3" t="s">
         <v>116</v>

</xml_diff>

<commit_message>
comments on FiNRT enhancement.
</commit_message>
<xml_diff>
--- a/doc/LitReview/TyndallLab/practice_reduction_estimates.xlsx
+++ b/doc/LitReview/TyndallLab/practice_reduction_estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnel\Documents\Project\G2G_supplyshed\doc\LitReview\TyndallLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DF8A1B-27DD-4D51-BD70-3793AFA0C4FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD657290-5126-4ECA-9885-70EC3BFC6088}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22185" windowHeight="12000" activeTab="2" xr2:uid="{2B4A4EA7-2393-4A3B-BE3A-A25348E227CC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22185" windowHeight="12000" activeTab="12" xr2:uid="{2B4A4EA7-2393-4A3B-BE3A-A25348E227CC}"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="13" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="122">
   <si>
     <t>Nutrient Removal Wetland</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t>conservation cover; TN; TSS; ChlA</t>
+  </si>
+  <si>
+    <t>error</t>
   </si>
 </sst>
 </file>
@@ -1105,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F7C739-06E6-4D7B-B2DD-AC136A1D2BAA}">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:R2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,8 +1487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FC7F79-CEB3-432E-A3AB-3A5236BDCD48}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1777,10 +1780,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{290E9E06-2429-438E-A13C-0C2CC43C98C0}">
-  <dimension ref="A1:R39"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1791,10 +1794,12 @@
     <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1818,25 +1823,28 @@
         <v>16</v>
       </c>
       <c r="M1" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
@@ -1871,8 +1879,9 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" s="4"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1885,31 +1894,31 @@
       <c r="L3">
         <v>52</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
     </row>

</xml_diff>